<commit_message>
added new tcs and updated pom
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmaheshw\PycharmProjects\appium_practice_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88A3AFF-B958-4C4F-99E9-E067E3E60780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70C1901-9896-4F65-BCDC-7F8BEBF7B026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +60,14 @@
       <sz val="16"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -106,10 +114,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -121,9 +130,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20" x14ac:dyDescent="0.4"/>
@@ -424,7 +437,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4">
@@ -432,8 +445,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B08FFB8B-E799-47C6-900C-9E636674C2EA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -441,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8E7743-FAC3-4F6A-A9AF-050DF42DD4C0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>